<commit_message>
Added total wait per year for campaign graph 10x+ Better run time for operations and campaigns result generation Fixed errors
</commit_message>
<xml_diff>
--- a/resources/Limit.xlsx
+++ b/resources/Limit.xlsx
@@ -21,6 +21,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>TheH(°N)/Tp(s)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,13 +348,16 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">

</xml_diff>

<commit_message>
A lot of changes: added TotalUnoperableSlotsMonthly graph logic fixes
</commit_message>
<xml_diff>
--- a/resources/Limit.xlsx
+++ b/resources/Limit.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="List2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,16 +25,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>TheH(°N)/Tp(s)</t>
+  </si>
+  <si>
+    <t>Tp/Dir</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,16 +46,34 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -59,15 +81,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Default" xfId="1"/>
     <cellStyle name="Navadno" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -345,18 +408,782 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>22.5</v>
+      </c>
+      <c r="D1" s="2">
+        <v>45</v>
+      </c>
+      <c r="E1" s="2">
+        <v>67.5</v>
+      </c>
+      <c r="F1" s="2">
+        <v>90</v>
+      </c>
+      <c r="G1" s="2">
+        <v>112.5</v>
+      </c>
+      <c r="H1" s="2">
+        <v>135</v>
+      </c>
+      <c r="I1" s="2">
+        <v>157.5</v>
+      </c>
+      <c r="J1" s="2">
+        <v>180</v>
+      </c>
+      <c r="K1" s="2">
+        <f t="shared" ref="K1:Q1" si="0">J1+22.5</f>
+        <v>202.5</v>
+      </c>
+      <c r="L1" s="2">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="M1" s="2">
+        <f t="shared" si="0"/>
+        <v>247.5</v>
+      </c>
+      <c r="N1" s="2">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="O1" s="2">
+        <f t="shared" si="0"/>
+        <v>292.5</v>
+      </c>
+      <c r="P1" s="2">
+        <f t="shared" si="0"/>
+        <v>315</v>
+      </c>
+      <c r="Q1" s="2">
+        <f t="shared" si="0"/>
+        <v>337.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4">
+        <v>100</v>
+      </c>
+      <c r="C2" s="4">
+        <v>100</v>
+      </c>
+      <c r="D2" s="4">
+        <v>100</v>
+      </c>
+      <c r="E2" s="4">
+        <v>100</v>
+      </c>
+      <c r="F2" s="4">
+        <v>100</v>
+      </c>
+      <c r="G2" s="4">
+        <v>100</v>
+      </c>
+      <c r="H2" s="4">
+        <v>100</v>
+      </c>
+      <c r="I2" s="4">
+        <v>100</v>
+      </c>
+      <c r="J2" s="4">
+        <v>100</v>
+      </c>
+      <c r="K2" s="4">
+        <v>100</v>
+      </c>
+      <c r="L2" s="4">
+        <v>100</v>
+      </c>
+      <c r="M2" s="4">
+        <v>100</v>
+      </c>
+      <c r="N2" s="4">
+        <v>100</v>
+      </c>
+      <c r="O2" s="4">
+        <v>100</v>
+      </c>
+      <c r="P2" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="1">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>100</v>
+      </c>
+      <c r="C3" s="4">
+        <v>100</v>
+      </c>
+      <c r="D3" s="4">
+        <v>100</v>
+      </c>
+      <c r="E3" s="4">
+        <v>100</v>
+      </c>
+      <c r="F3" s="4">
+        <v>100</v>
+      </c>
+      <c r="G3" s="4">
+        <v>100</v>
+      </c>
+      <c r="H3" s="4">
+        <v>100</v>
+      </c>
+      <c r="I3" s="4">
+        <v>100</v>
+      </c>
+      <c r="J3" s="4">
+        <v>100</v>
+      </c>
+      <c r="K3" s="4">
+        <v>100</v>
+      </c>
+      <c r="L3" s="4">
+        <v>100</v>
+      </c>
+      <c r="M3" s="4">
+        <v>100</v>
+      </c>
+      <c r="N3" s="4">
+        <v>100</v>
+      </c>
+      <c r="O3" s="4">
+        <v>100</v>
+      </c>
+      <c r="P3" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="1">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4">
+        <v>100</v>
+      </c>
+      <c r="C4" s="4">
+        <v>100</v>
+      </c>
+      <c r="D4" s="4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="4">
+        <v>100</v>
+      </c>
+      <c r="F4" s="4">
+        <v>100</v>
+      </c>
+      <c r="G4" s="4">
+        <v>100</v>
+      </c>
+      <c r="H4" s="4">
+        <v>100</v>
+      </c>
+      <c r="I4" s="4">
+        <v>100</v>
+      </c>
+      <c r="J4" s="4">
+        <v>100</v>
+      </c>
+      <c r="K4" s="4">
+        <v>100</v>
+      </c>
+      <c r="L4" s="4">
+        <v>100</v>
+      </c>
+      <c r="M4" s="4">
+        <v>100</v>
+      </c>
+      <c r="N4" s="4">
+        <v>100</v>
+      </c>
+      <c r="O4" s="4">
+        <v>100</v>
+      </c>
+      <c r="P4" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="1">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4">
+        <v>100</v>
+      </c>
+      <c r="C5" s="4">
+        <v>100</v>
+      </c>
+      <c r="D5" s="4">
+        <v>100</v>
+      </c>
+      <c r="E5" s="4">
+        <v>100</v>
+      </c>
+      <c r="F5" s="4">
+        <v>100</v>
+      </c>
+      <c r="G5" s="4">
+        <v>100</v>
+      </c>
+      <c r="H5" s="4">
+        <v>100</v>
+      </c>
+      <c r="I5" s="4">
+        <v>100</v>
+      </c>
+      <c r="J5" s="4">
+        <v>100</v>
+      </c>
+      <c r="K5" s="4">
+        <v>100</v>
+      </c>
+      <c r="L5" s="4">
+        <v>100</v>
+      </c>
+      <c r="M5" s="4">
+        <v>100</v>
+      </c>
+      <c r="N5" s="4">
+        <v>100</v>
+      </c>
+      <c r="O5" s="4">
+        <v>100</v>
+      </c>
+      <c r="P5" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="1">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4">
+        <v>100</v>
+      </c>
+      <c r="C6" s="4">
+        <v>100</v>
+      </c>
+      <c r="D6" s="4">
+        <v>100</v>
+      </c>
+      <c r="E6" s="4">
+        <v>100</v>
+      </c>
+      <c r="F6" s="4">
+        <v>100</v>
+      </c>
+      <c r="G6" s="4">
+        <v>100</v>
+      </c>
+      <c r="H6" s="4">
+        <v>100</v>
+      </c>
+      <c r="I6" s="4">
+        <v>100</v>
+      </c>
+      <c r="J6" s="4">
+        <v>100</v>
+      </c>
+      <c r="K6" s="4">
+        <v>100</v>
+      </c>
+      <c r="L6" s="4">
+        <v>100</v>
+      </c>
+      <c r="M6" s="4">
+        <v>100</v>
+      </c>
+      <c r="N6" s="4">
+        <v>100</v>
+      </c>
+      <c r="O6" s="4">
+        <v>100</v>
+      </c>
+      <c r="P6" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="1">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4">
+        <v>100</v>
+      </c>
+      <c r="C7" s="4">
+        <v>100</v>
+      </c>
+      <c r="D7" s="4">
+        <v>100</v>
+      </c>
+      <c r="E7" s="4">
+        <v>100</v>
+      </c>
+      <c r="F7" s="4">
+        <v>100</v>
+      </c>
+      <c r="G7" s="4">
+        <v>100</v>
+      </c>
+      <c r="H7" s="4">
+        <v>100</v>
+      </c>
+      <c r="I7" s="4">
+        <v>100</v>
+      </c>
+      <c r="J7" s="4">
+        <v>100</v>
+      </c>
+      <c r="K7" s="4">
+        <v>100</v>
+      </c>
+      <c r="L7" s="4">
+        <v>100</v>
+      </c>
+      <c r="M7" s="4">
+        <v>100</v>
+      </c>
+      <c r="N7" s="4">
+        <v>100</v>
+      </c>
+      <c r="O7" s="4">
+        <v>100</v>
+      </c>
+      <c r="P7" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="1">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4">
+        <v>100</v>
+      </c>
+      <c r="C8" s="4">
+        <v>100</v>
+      </c>
+      <c r="D8" s="4">
+        <v>100</v>
+      </c>
+      <c r="E8" s="4">
+        <v>100</v>
+      </c>
+      <c r="F8" s="4">
+        <v>100</v>
+      </c>
+      <c r="G8" s="4">
+        <v>100</v>
+      </c>
+      <c r="H8" s="4">
+        <v>100</v>
+      </c>
+      <c r="I8" s="4">
+        <v>100</v>
+      </c>
+      <c r="J8" s="4">
+        <v>100</v>
+      </c>
+      <c r="K8" s="4">
+        <v>100</v>
+      </c>
+      <c r="L8" s="4">
+        <v>100</v>
+      </c>
+      <c r="M8" s="4">
+        <v>100</v>
+      </c>
+      <c r="N8" s="4">
+        <v>100</v>
+      </c>
+      <c r="O8" s="4">
+        <v>100</v>
+      </c>
+      <c r="P8" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="1">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4">
+        <v>100</v>
+      </c>
+      <c r="C9" s="4">
+        <v>100</v>
+      </c>
+      <c r="D9" s="4">
+        <v>100</v>
+      </c>
+      <c r="E9" s="4">
+        <v>100</v>
+      </c>
+      <c r="F9" s="4">
+        <v>100</v>
+      </c>
+      <c r="G9" s="4">
+        <v>100</v>
+      </c>
+      <c r="H9" s="4">
+        <v>100</v>
+      </c>
+      <c r="I9" s="4">
+        <v>100</v>
+      </c>
+      <c r="J9" s="4">
+        <v>100</v>
+      </c>
+      <c r="K9" s="4">
+        <v>100</v>
+      </c>
+      <c r="L9" s="4">
+        <v>100</v>
+      </c>
+      <c r="M9" s="4">
+        <v>100</v>
+      </c>
+      <c r="N9" s="4">
+        <v>100</v>
+      </c>
+      <c r="O9" s="4">
+        <v>100</v>
+      </c>
+      <c r="P9" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="1">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4">
+        <v>100</v>
+      </c>
+      <c r="C10" s="4">
+        <v>100</v>
+      </c>
+      <c r="D10" s="4">
+        <v>100</v>
+      </c>
+      <c r="E10" s="4">
+        <v>100</v>
+      </c>
+      <c r="F10" s="4">
+        <v>100</v>
+      </c>
+      <c r="G10" s="4">
+        <v>100</v>
+      </c>
+      <c r="H10" s="4">
+        <v>100</v>
+      </c>
+      <c r="I10" s="4">
+        <v>100</v>
+      </c>
+      <c r="J10" s="4">
+        <v>100</v>
+      </c>
+      <c r="K10" s="4">
+        <v>100</v>
+      </c>
+      <c r="L10" s="4">
+        <v>100</v>
+      </c>
+      <c r="M10" s="4">
+        <v>100</v>
+      </c>
+      <c r="N10" s="4">
+        <v>100</v>
+      </c>
+      <c r="O10" s="4">
+        <v>100</v>
+      </c>
+      <c r="P10" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="1">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4">
+        <v>100</v>
+      </c>
+      <c r="C11" s="4">
+        <v>100</v>
+      </c>
+      <c r="D11" s="4">
+        <v>100</v>
+      </c>
+      <c r="E11" s="4">
+        <v>100</v>
+      </c>
+      <c r="F11" s="4">
+        <v>100</v>
+      </c>
+      <c r="G11" s="4">
+        <v>100</v>
+      </c>
+      <c r="H11" s="4">
+        <v>100</v>
+      </c>
+      <c r="I11" s="4">
+        <v>100</v>
+      </c>
+      <c r="J11" s="4">
+        <v>100</v>
+      </c>
+      <c r="K11" s="4">
+        <v>100</v>
+      </c>
+      <c r="L11" s="4">
+        <v>100</v>
+      </c>
+      <c r="M11" s="4">
+        <v>100</v>
+      </c>
+      <c r="N11" s="4">
+        <v>100</v>
+      </c>
+      <c r="O11" s="4">
+        <v>100</v>
+      </c>
+      <c r="P11" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="1">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4">
+        <v>100</v>
+      </c>
+      <c r="C12" s="4">
+        <v>100</v>
+      </c>
+      <c r="D12" s="4">
+        <v>100</v>
+      </c>
+      <c r="E12" s="4">
+        <v>100</v>
+      </c>
+      <c r="F12" s="4">
+        <v>100</v>
+      </c>
+      <c r="G12" s="4">
+        <v>100</v>
+      </c>
+      <c r="H12" s="4">
+        <v>100</v>
+      </c>
+      <c r="I12" s="4">
+        <v>100</v>
+      </c>
+      <c r="J12" s="4">
+        <v>100</v>
+      </c>
+      <c r="K12" s="4">
+        <v>100</v>
+      </c>
+      <c r="L12" s="4">
+        <v>100</v>
+      </c>
+      <c r="M12" s="4">
+        <v>100</v>
+      </c>
+      <c r="N12" s="4">
+        <v>100</v>
+      </c>
+      <c r="O12" s="4">
+        <v>100</v>
+      </c>
+      <c r="P12" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="1">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4">
+        <v>100</v>
+      </c>
+      <c r="C13" s="4">
+        <v>100</v>
+      </c>
+      <c r="D13" s="4">
+        <v>100</v>
+      </c>
+      <c r="E13" s="4">
+        <v>100</v>
+      </c>
+      <c r="F13" s="4">
+        <v>100</v>
+      </c>
+      <c r="G13" s="4">
+        <v>100</v>
+      </c>
+      <c r="H13" s="4">
+        <v>100</v>
+      </c>
+      <c r="I13" s="4">
+        <v>100</v>
+      </c>
+      <c r="J13" s="4">
+        <v>100</v>
+      </c>
+      <c r="K13" s="4">
+        <v>100</v>
+      </c>
+      <c r="L13" s="4">
+        <v>100</v>
+      </c>
+      <c r="M13" s="4">
+        <v>100</v>
+      </c>
+      <c r="N13" s="4">
+        <v>100</v>
+      </c>
+      <c r="O13" s="4">
+        <v>100</v>
+      </c>
+      <c r="P13" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="3">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4">
+        <v>100</v>
+      </c>
+      <c r="C14" s="4">
+        <v>100</v>
+      </c>
+      <c r="D14" s="4">
+        <v>100</v>
+      </c>
+      <c r="E14" s="4">
+        <v>100</v>
+      </c>
+      <c r="F14" s="4">
+        <v>100</v>
+      </c>
+      <c r="G14" s="4">
+        <v>100</v>
+      </c>
+      <c r="H14" s="4">
+        <v>100</v>
+      </c>
+      <c r="I14" s="4">
+        <v>100</v>
+      </c>
+      <c r="J14" s="4">
+        <v>100</v>
+      </c>
+      <c r="K14" s="4">
+        <v>100</v>
+      </c>
+      <c r="L14" s="4">
+        <v>100</v>
+      </c>
+      <c r="M14" s="4">
+        <v>100</v>
+      </c>
+      <c r="N14" s="4">
+        <v>100</v>
+      </c>
+      <c r="O14" s="4">
+        <v>100</v>
+      </c>
+      <c r="P14" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -388,7 +1215,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -420,7 +1247,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -452,7 +1279,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -484,7 +1311,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -516,7 +1343,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>6</v>
       </c>
@@ -548,7 +1375,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>8</v>
       </c>
@@ -580,7 +1407,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>10</v>
       </c>
@@ -612,7 +1439,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>12</v>
       </c>

</xml_diff>